<commit_message>
GHS hazards addes, format changed to be more readable, GUI front end could be added, and more improvement could be added, almost finished
</commit_message>
<xml_diff>
--- a/OutputReports/MSDS_report.xlsx
+++ b/OutputReports/MSDS_report.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lianghao/Desktop/MSDS_Generator_py/OutputReports/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF36946-28E6-0C40-9DFB-DD617302BF6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHMD16-Lab1-SoilAnalysis" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Compound</t>
   </si>
@@ -28,22 +34,40 @@
     <t>First Aids</t>
   </si>
   <si>
-    <t>Sodium chlorid</t>
-  </si>
-  <si>
-    <t>Boiling Point: 2575 °F at 760 mm Hg (NTP, 1992);Melting Point: 1474 °F (NTP, 1992);solubility: greater than or equal to 100 mg/mL at 68° F (NTP, 1992);Density: 2.165 at 77 °F (NTP, 1992);</t>
-  </si>
-  <si>
-    <t>The rare inadvertent intravascular administration or rapid intravascular absorption of hypertonic sodium chloride can cause a shift of tissue fluids into the vascular bed, resulting in hypervolemia, electrolyte disturbances, circulatory failure, pulmonary embolism, or augmented hypertension. ( toxnet</t>
-  </si>
-  <si>
-    <t>EYES: First check the victim for contact lenses and remove if present. Flush victim's eyes with water or normal saline solution for 20 to 30 minutes while simultaneously calling a hospital or poison control center. Do not put any ointments, oils, or medication in the victim's eyes without specific instructions from a physician. IMMEDIATELY transport the victim after flushing eyes to a hospital even if no symptoms (such as redness or irritation) develop. SKIN: IMMEDIATELY flood affected skin with water while removing and isolating all contaminated clothing. Gently wash all affected skin areas thoroughly with soap and water. If symptoms such as redness or irritation develop, IMMEDIATELY call a physician and be prepared to transport the victim to a hospital for treatment. INHALATION: IMMEDIATELY leave the contaminated area; take deep breaths of fresh air. If symptoms (such as wheezing, coughing, shortness of breath, or burning in the mouth, throat, or chest) develop, call a physician and be prepared to transport the victim to a hospital. Provide proper respiratory protection to rescuers entering an unknown atmosphere. Whenever possible, Self-Contained Breathing Apparatus (SCBA) should be used; if not available, use a level of protection greater than or equal to that advised under Protective Clothing. INGESTION: DO NOT INDUCE VOMITING. If the victim is conscious and not convulsing, give 1 or 2 glasses of water to dilute the chemical and IMMEDIATELY call a hospital or poison control center. Be prepared to transport the victim to a hospital if advised by a physician. If the victim is convulsing or unconscious, do not give anything by mouth, ensure that the victim's airway is open and lay the victim on his/her side with the head lower than the body. DO NOT INDUCE VOMITING. IMMEDIATELY transport the victim to a hospital. (NTP, 1992)</t>
+    <t>Hydrochloric acid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ordor: Pungent, irritating odor;
+Boiling Point: 123 °F at 760 mm Hg (USCG, 1999);
+Melting Point: -174.6 °F (Melting point is -13.7° F for a 39.17% weight/weight solution.) (EPA, 1998);
+solubility: 82.3 g/100 g at 32° F (NTP, 1992);
+Density: 1.05 at 59 °F for 10.17% weight/weight solution (EPA, 1998);
+</t>
+  </si>
+  <si>
+    <t>H314: Causes severe skin burns and eye damage [Danger Skin corrosion/irritation]
+H331: Toxic if inhaled [Danger Acute toxicity, inhalation]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inhalation: Fresh air, rest. Half-upright position. Artificial respiration may be needed. Refer immediately for medical attention.
+skin: Wear protective gloves when administering first aid. First rinse with plenty of water for at least 15 minutes, then remove contaminated clothes and rinse again. Refer immediately for medical attention.
+eye: Rinse with plenty of water for several minutes (remove contact lenses if easily possible). Refer immediately for medical attention.
+</t>
   </si>
   <si>
     <t>Calcium carbonate</t>
   </si>
   <si>
-    <t>ordor: Odorless;Boiling Point: Decomposes (NIOSH, 2016);Melting Point: 1517 to 2442 °F (Decomposes) (NIOSH, 2016);solubility: 0.001 % (NIOSH, 2016);Density: 2.7 to 2.95 (NIOSH, 2016);</t>
+    <t xml:space="preserve">ordor: Odorless;
+Boiling Point: Decomposes (NIOSH, 2016);
+Melting Point: 1517 to 2442 °F (Decomposes) (NIOSH, 2016);
+solubility: 0.001 % (NIOSH, 2016);
+Density: 2.7 to 2.95 (NIOSH, 2016);
+</t>
+  </si>
+  <si>
+    <t>Not Classified
+Reported as not meeting GHS hazard criteria by 3306 of 3614 companies (only ~ 8.5% companies provided GHS information). For more detailed information, please visit ECHA C&amp;L website</t>
   </si>
   <si>
     <t xml:space="preserve">inhalation: Fresh air.
@@ -53,31 +77,35 @@
 </t>
   </si>
   <si>
-    <t>Calcium chloride</t>
-  </si>
-  <si>
-    <t>Boiling Point: 1670 °C;Melting Point: 782 °C;solubility: 0.745 g/mL (at 20 °C);Density: 2.15 at 68 °F (USCG, 1999);</t>
-  </si>
-  <si>
-    <t>Too rapid injection may produce lowering of blood pressure and cardiac syncope. Persistent hypercalcemia from overdosage of calcium is unlikely because of rapid excretion.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inhalation: Fresh air, rest. Refer for medical attention.
-skin: Remove contaminated clothes. Rinse skin with plenty of water or shower. Refer immediately for medical attention.
-eye: Rinse with plenty of water for several minutes (remove contact lenses if easily possible). Refer immediately for medical attention.
-ingestion: Rinse mouth. Do NOT induce vomiting. Give one or two glasses of water to drink. Refer immediately for medical attention.
+    <t>Sodium chloride</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boiling Point: 2575 °F at 760 mm Hg (NTP, 1992);
+Melting Point: 1474 °F (NTP, 1992);
+solubility: greater than or equal to 100 mg/mL at 68° F (NTP, 1992);
+Density: 2.165 at 77 °F (NTP, 1992);
 </t>
+  </si>
+  <si>
+    <t>Aggregated GHS information provided by 2341 companies from 13 notifications to the ECHA C&amp;L Inventory.
+Reported as not meeting GHS hazard criteria by 1699 of 2341 companies. For more detailed information, please visit ECHA C&amp;L website
+Of the 9 notification(s) provided by 642 of 2341 companies with hazard statement code(s):
+H319 (100%): Causes serious eye irritation [Warning Serious eye damage/eye irritation]
+Information may vary between notifications depending on impurities, additives, and other factors. The percentage value in parenthesis indicates the notified classification ratio from companies that provide hazard codes. Only hazard codes with percentage values above 10% are shown.</t>
+  </si>
+  <si>
+    <t>EYES: First check the victim for contact lenses and remove if present. Flush victim's eyes with water or normal saline solution for 20 to 30 minutes while simultaneously calling a hospital or poison control center. Do not put any ointments, oils, or medication in the victim's eyes without specific instructions from a physician. IMMEDIATELY transport the victim after flushing eyes to a hospital even if no symptoms (such as redness or irritation) develop. SKIN: IMMEDIATELY flood affected skin with water while removing and isolating all contaminated clothing. Gently wash all affected skin areas thoroughly with soap and water. If symptoms such as redness or irritation develop, IMMEDIATELY call a physician and be prepared to transport the victim to a hospital for treatment. INHALATION: IMMEDIATELY leave the contaminated area; take deep breaths of fresh air. If symptoms (such as wheezing, coughing, shortness of breath, or burning in the mouth, throat, or chest) develop, call a physician and be prepared to transport the victim to a hospital. Provide proper respiratory protection to rescuers entering an unknown atmosphere. Whenever possible, Self-Contained Breathing Apparatus (SCBA) should be used; if not available, use a level of protection greater than or equal to that advised under Protective Clothing. INGESTION: DO NOT INDUCE VOMITING. If the victim is conscious and not convulsing, give 1 or 2 glasses of water to dilute the chemical and IMMEDIATELY call a hospital or poison control center. Be prepared to transport the victim to a hospital if advised by a physician. If the victim is convulsing or unconscious, do not give anything by mouth, ensure that the victim's airway is open and lay the victim on his/her side with the head lower than the body. DO NOT INDUCE VOMITING. IMMEDIATELY transport the victim to a hospital. (NTP, 1992)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -85,8 +113,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -110,20 +145,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -165,7 +219,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -197,9 +251,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -231,6 +303,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -406,67 +496,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="18" style="3" customWidth="1"/>
+    <col min="2" max="2" width="69.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="64.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="81.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="15">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" ht="120">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" ht="105">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:4" ht="370">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="4" t="s">
         <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>